<commit_message>
improved logging and screenshot taking
</commit_message>
<xml_diff>
--- a/TestData/Test Data.xlsx
+++ b/TestData/Test Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddharth\Google Drive\PycharmProjects\nopAdminSelenium\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE2A82E-6ED4-4792-BB4F-800C60507D20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F62BD9-4221-4E06-9DF7-ED3C39EAFBDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>cold@hotmail.com</t>
+  </si>
+  <si>
+    <t>admin@yourstore.com</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -670,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5672C3A0-542C-4C10-8138-28654EF95CCA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,6 +744,17 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Commit from new laptop
</commit_message>
<xml_diff>
--- a/TestData/Test Data.xlsx
+++ b/TestData/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddharth\Google Drive\PycharmProjects\nopAdminSelenium\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FF2EA1-7A10-43F8-9D3C-DB42FC7CDC15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E87FAFC-5425-430A-A1A9-75C59BFD2A4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>cold@hotmail.com</t>
+  </si>
+  <si>
+    <t>admin@yourstore.com</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -673,7 +679,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:H26"/>
+  <dimension ref="A3:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,6 +1429,19 @@
         <v>C_DEAL_ID_NUM = 'Deal ID Num'</v>
       </c>
     </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>